<commit_message>
rewrite of control state machine.  Example now performs multiple additions
</commit_message>
<xml_diff>
--- a/docs/control.xlsx
+++ b/docs/control.xlsx
@@ -442,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,10 +520,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -607,10 +603,10 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="G43" activeCellId="0" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.49"/>
@@ -1240,13 +1236,13 @@
       <c r="F18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="7" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="19" t="s">
@@ -1456,7 +1452,7 @@
       <c r="H23" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="7" t="s">
         <v>49</v>
       </c>
       <c r="J23" s="19" t="s">
@@ -1787,13 +1783,13 @@
       <c r="F30" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="7" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="20" t="s">
+      <c r="I30" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J30" s="19" t="s">

</xml_diff>